<commit_message>
Added indesign test cases (from Christy) and updated pdf_testcases.xlsx to reflect these changes.
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@57 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/pdf_testcases.xlsx
+++ b/testcases/pdf_testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t>Filename</t>
   </si>
@@ -147,9 +147,6 @@
     <t>starbucks_textonly-primopdf</t>
   </si>
   <si>
-    <t>generated by MSWord's embedded "save as PDF"</t>
-  </si>
-  <si>
     <t>generated by primopdf plugin through MSWord</t>
   </si>
   <si>
@@ -166,6 +163,39 @@
   </si>
   <si>
     <t>tagged figure</t>
+  </si>
+  <si>
+    <t>indesign-form</t>
+  </si>
+  <si>
+    <t>indesign-image</t>
+  </si>
+  <si>
+    <t>indesign-tables</t>
+  </si>
+  <si>
+    <t>indesign-text-only</t>
+  </si>
+  <si>
+    <t>created in InDesign CS3</t>
+  </si>
+  <si>
+    <t>&lt;document&gt;, &lt;article&gt;, &lt;story&gt;</t>
+  </si>
+  <si>
+    <t>&lt;document&gt;, &lt;article&gt;, &lt;figure&gt;</t>
+  </si>
+  <si>
+    <t>text, forms</t>
+  </si>
+  <si>
+    <t>image only</t>
+  </si>
+  <si>
+    <t>blank &lt;Document&gt; &lt;/Document&gt; xml file</t>
+  </si>
+  <si>
+    <t>generated by MSWord's "save as PDF"</t>
   </si>
 </sst>
 </file>
@@ -530,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,7 +574,7 @@
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -591,272 +621,275 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>39</v>
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
@@ -865,89 +898,178 @@
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>39</v>
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+      <c r="D22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating latest version of pdf_testcases.xlsx to repository
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@64 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/pdf_testcases.xlsx
+++ b/testcases/pdf_testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>Filename</t>
   </si>
@@ -135,9 +135,6 @@
     <t>tagged text</t>
   </si>
   <si>
-    <t>invalid xml file (due to invalid characters such as spaces in a tag ie: &lt;heading 1&gt;); otherwise valid</t>
-  </si>
-  <si>
     <t>Features</t>
   </si>
   <si>
@@ -196,6 +193,36 @@
   </si>
   <si>
     <t>generated by MSWord's "save as PDF"</t>
+  </si>
+  <si>
+    <t>(fuller xml than itext. See file for more details.)</t>
+  </si>
+  <si>
+    <t>Same*</t>
+  </si>
+  <si>
+    <t>headings contain id names, otherwise same*</t>
+  </si>
+  <si>
+    <t>* = all Adobe Acrobat xml outputs have information about the xml/pdf file that itext does not create.</t>
+  </si>
+  <si>
+    <t>invalid xml file (due to invalid characters such as spaces in a tag ie: &lt;heading 1&gt; is translated to &lt;heading#201&gt;); otherwise valid</t>
+  </si>
+  <si>
+    <t>Text next to outline bullets or checkboxes is not included in the itext vers.</t>
+  </si>
+  <si>
+    <t>Acrobat Pro Output Comparisons to iText</t>
+  </si>
+  <si>
+    <t>contains filename of figure (itext does not)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>contains full tagging</t>
   </si>
 </sst>
 </file>
@@ -560,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -571,13 +598,14 @@
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +613,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
@@ -597,10 +625,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -619,59 +650,71 @@
       <c r="F2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>27</v>
@@ -683,18 +726,21 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -706,13 +752,16 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -731,8 +780,14 @@
       <c r="F7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -752,10 +807,13 @@
         <v>38</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -774,8 +832,14 @@
       <c r="F9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -794,8 +858,14 @@
       <c r="F10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -812,10 +882,16 @@
         <v>3</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -834,39 +910,48 @@
       <c r="F12" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
@@ -878,15 +963,18 @@
         <v>37</v>
       </c>
       <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>
@@ -900,13 +988,16 @@
       <c r="F15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>15</v>
@@ -924,10 +1015,13 @@
         <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -946,8 +1040,14 @@
       <c r="F17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -966,11 +1066,14 @@
       <c r="F18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -989,8 +1092,14 @@
       <c r="F19" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="G19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1009,8 +1118,14 @@
       <c r="F20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
@@ -1027,10 +1142,16 @@
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1049,8 +1170,14 @@
       <c r="F22" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1197,15 @@
         <v>37</v>
       </c>
       <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>